<commit_message>
Search Skll -> Filter, user and any string
</commit_message>
<xml_diff>
--- a/SpecflowPM.Tests/ExcelTestData/SearchCategory.xlsx
+++ b/SpecflowPM.Tests/ExcelTestData/SearchCategory.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Pinky Sindhu\Desktop\Industry Connect\Industry Connect\Internship\Task 3\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Pinky Sindhu\Desktop\Industry Connect\Industry Connect\Internship\Task 3\ProjectMars.QA\SpecflowPM.Tests\ExcelTestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{15D03BCA-749B-4A26-BECD-86E4264E0BCD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6DEEECD0-4BDC-4D20-863C-7502911D37CA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-96" yWindow="-96" windowWidth="19392" windowHeight="10392" xr2:uid="{A3C116B1-579C-403F-9F81-D78A60AE9A2F}"/>
+    <workbookView xWindow="-96" yWindow="-96" windowWidth="19392" windowHeight="10392" activeTab="1" xr2:uid="{A3C116B1-579C-403F-9F81-D78A60AE9A2F}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -32,12 +32,156 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="2">
-  <si>
-    <t>Category</t>
-  </si>
-  <si>
-    <t>SubCategory</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="50">
+  <si>
+    <t>CategoryIndex</t>
+  </si>
+  <si>
+    <t>SubCatCount</t>
+  </si>
+  <si>
+    <t>| subcat1                  |</t>
+  </si>
+  <si>
+    <t>| Logo Design              |</t>
+  </si>
+  <si>
+    <t>| Book Album covers        |</t>
+  </si>
+  <si>
+    <t>| Flyers Brochures16       |</t>
+  </si>
+  <si>
+    <t>| Web Mobile Design        |</t>
+  </si>
+  <si>
+    <t>| Search Display Marketing |</t>
+  </si>
+  <si>
+    <t>| subcat2                  |</t>
+  </si>
+  <si>
+    <t>| Social Media Marketing   |</t>
+  </si>
+  <si>
+    <t>| Content Marketing        |</t>
+  </si>
+  <si>
+    <t>| Video Marketing          |</t>
+  </si>
+  <si>
+    <t>| Email Marketing          |</t>
+  </si>
+  <si>
+    <t>| subcat3               |</t>
+  </si>
+  <si>
+    <t>| Resumes Cover Letters |</t>
+  </si>
+  <si>
+    <t>| Proof Reading Editing |</t>
+  </si>
+  <si>
+    <t>| Translation           |</t>
+  </si>
+  <si>
+    <t>| Creative Writing      |</t>
+  </si>
+  <si>
+    <t>| Business Copywriting  |</t>
+  </si>
+  <si>
+    <t>| subcat4                 |</t>
+  </si>
+  <si>
+    <t>| Promotional Videos      |</t>
+  </si>
+  <si>
+    <t>| Editing Post Production |</t>
+  </si>
+  <si>
+    <t>| Lyric Music Videos      |</t>
+  </si>
+  <si>
+    <t xml:space="preserve">| Other                   |  </t>
+  </si>
+  <si>
+    <t>| subcat5                |</t>
+  </si>
+  <si>
+    <t>| Mixing Mastering       |</t>
+  </si>
+  <si>
+    <t>| Voice Over             |</t>
+  </si>
+  <si>
+    <t>| Song Writers Composers |</t>
+  </si>
+  <si>
+    <t>| Other                  |</t>
+  </si>
+  <si>
+    <t>| subcat6               |</t>
+  </si>
+  <si>
+    <t>| WordPress             |</t>
+  </si>
+  <si>
+    <t>| Web Mobile App        |</t>
+  </si>
+  <si>
+    <t>| Data Analysis Reports |</t>
+  </si>
+  <si>
+    <t>| QA                    |</t>
+  </si>
+  <si>
+    <t>| Databases             |</t>
+  </si>
+  <si>
+    <t>| Other                 |</t>
+  </si>
+  <si>
+    <t>| subcat7              |</t>
+  </si>
+  <si>
+    <t>| Business Tips        |</t>
+  </si>
+  <si>
+    <t>| Presentations        |</t>
+  </si>
+  <si>
+    <t>| Market Advice        |</t>
+  </si>
+  <si>
+    <t>| Legal Consulting     |</t>
+  </si>
+  <si>
+    <t>| Financial Consulting |</t>
+  </si>
+  <si>
+    <t>| Other                |</t>
+  </si>
+  <si>
+    <t>| subcat8                   |</t>
+  </si>
+  <si>
+    <t>| Online Lessons            |</t>
+  </si>
+  <si>
+    <t>| Relationship Advice       |</t>
+  </si>
+  <si>
+    <t>| Astrology                 |</t>
+  </si>
+  <si>
+    <t>| Health Nutrition  Fitness |</t>
+  </si>
+  <si>
+    <t>| Gaming                    |</t>
+  </si>
+  <si>
+    <t>| Other                     |</t>
   </si>
 </sst>
 </file>
@@ -389,14 +533,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{86FBAE02-E5B5-4C4C-835D-E2BEB000F350}">
-  <dimension ref="A1:B5"/>
+  <dimension ref="A1:B9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L12" sqref="L12"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B1" sqref="B1:B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
+    <col min="1" max="1" width="16.47265625" customWidth="1"/>
     <col min="2" max="2" width="10.68359375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -440,62 +585,221 @@
         <v>4</v>
       </c>
     </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="B7">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A8">
+        <v>7</v>
+      </c>
+      <c r="B8">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A9">
+        <v>8</v>
+      </c>
+      <c r="B9">
+        <v>6</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BF211A83-DE91-4C92-93DE-94565104E84A}">
-  <dimension ref="A1:B5"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C65DC9F3-6B83-4638-A9EF-647B1CBFA8F7}">
+  <dimension ref="A1:H7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="N11" sqref="N11"/>
+    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
-    <col min="2" max="2" width="10.68359375" bestFit="1" customWidth="1"/>
+    <col min="1" max="2" width="23.3671875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="21.3671875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="21.734375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="22.83984375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="20.3671875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="18.9453125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="22.3671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="B1" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.55000000000000004">
-      <c r="A2">
-        <v>1</v>
-      </c>
-      <c r="B2">
+        <v>8</v>
+      </c>
+      <c r="C1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D1" t="s">
+        <v>19</v>
+      </c>
+      <c r="E1" t="s">
+        <v>24</v>
+      </c>
+      <c r="F1" t="s">
+        <v>29</v>
+      </c>
+      <c r="G1" t="s">
+        <v>36</v>
+      </c>
+      <c r="H1" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C2" t="s">
+        <v>14</v>
+      </c>
+      <c r="D2" t="s">
+        <v>20</v>
+      </c>
+      <c r="E2" t="s">
+        <v>25</v>
+      </c>
+      <c r="F2" t="s">
+        <v>30</v>
+      </c>
+      <c r="G2" t="s">
+        <v>37</v>
+      </c>
+      <c r="H2" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A3" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.55000000000000004">
-      <c r="A3">
-        <v>2</v>
-      </c>
-      <c r="B3">
+      <c r="B3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C3" t="s">
+        <v>15</v>
+      </c>
+      <c r="D3" t="s">
+        <v>21</v>
+      </c>
+      <c r="E3" t="s">
+        <v>26</v>
+      </c>
+      <c r="F3" t="s">
+        <v>31</v>
+      </c>
+      <c r="G3" t="s">
+        <v>38</v>
+      </c>
+      <c r="H3" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C4" t="s">
+        <v>16</v>
+      </c>
+      <c r="D4" t="s">
+        <v>22</v>
+      </c>
+      <c r="E4" t="s">
+        <v>27</v>
+      </c>
+      <c r="F4" t="s">
+        <v>32</v>
+      </c>
+      <c r="G4" t="s">
+        <v>39</v>
+      </c>
+      <c r="H4" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A5" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.55000000000000004">
-      <c r="A4">
-        <v>3</v>
-      </c>
-      <c r="B4">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.55000000000000004">
-      <c r="A5">
-        <v>4</v>
-      </c>
-      <c r="B5">
-        <v>6</v>
+      <c r="B5" t="s">
+        <v>12</v>
+      </c>
+      <c r="C5" t="s">
+        <v>17</v>
+      </c>
+      <c r="D5" t="s">
+        <v>23</v>
+      </c>
+      <c r="E5" t="s">
+        <v>28</v>
+      </c>
+      <c r="F5" t="s">
+        <v>33</v>
+      </c>
+      <c r="G5" t="s">
+        <v>40</v>
+      </c>
+      <c r="H5" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A6" t="s">
+        <v>7</v>
+      </c>
+      <c r="B6" t="s">
+        <v>7</v>
+      </c>
+      <c r="C6" t="s">
+        <v>18</v>
+      </c>
+      <c r="F6" t="s">
+        <v>34</v>
+      </c>
+      <c r="G6" t="s">
+        <v>41</v>
+      </c>
+      <c r="H6" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+      <c r="F7" t="s">
+        <v>35</v>
+      </c>
+      <c r="G7" t="s">
+        <v>42</v>
+      </c>
+      <c r="H7" t="s">
+        <v>49</v>
       </c>
     </row>
   </sheetData>

</xml_diff>